<commit_message>
add new lasso features
</commit_message>
<xml_diff>
--- a/gp/Ea_gp_models.xlsx
+++ b/gp/Ea_gp_models.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8836B4CF-CDE8-4F19-88A8-C9A74E42044D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="2715" windowWidth="23730" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="645" yWindow="2715" windowWidth="23730" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">Model </t>
   </si>
@@ -31,9 +30,6 @@
     <t>Model Expression</t>
   </si>
   <si>
-    <t>div(mul(X1, 0.566), div(X0, X1))</t>
-  </si>
-  <si>
     <t>X0</t>
   </si>
   <si>
@@ -46,43 +42,55 @@
     <t>Ebind</t>
   </si>
   <si>
-    <t>div(mul(0.602, X1), div(X0, sub(X1, 0.341)))</t>
-  </si>
-  <si>
-    <t>div(mul(0.563, X1), div(X0, X1))</t>
-  </si>
-  <si>
-    <t>div(mul(X1, 0.585), div(X0, X1))</t>
-  </si>
-  <si>
-    <t>mul(mul(0.581, X1), div(X1, X0))</t>
-  </si>
-  <si>
-    <t>Ea = 0.566*Ebind^2/Ec</t>
-  </si>
-  <si>
-    <t>Ea = 0.585*Ebind^2/Ec</t>
-  </si>
-  <si>
     <t>MAE (eV)</t>
   </si>
   <si>
     <t>RMSE (eV)</t>
   </si>
   <si>
-    <t>Ea = 0.602*Ebind^2/Ec -0.205 Ebind/Ec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ea = 0.581*Ebind^2/Ec </t>
-  </si>
-  <si>
-    <t>Ea = 0.563*Ebind^2/Ec</t>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>pearson r</t>
+  </si>
+  <si>
+    <t>div(mul(X1, X1), div(X0, 0.553))</t>
+  </si>
+  <si>
+    <t>Ea = 0.553*Ebind^2/Ec</t>
+  </si>
+  <si>
+    <t>mul(sub(X1, sqrt(X1)), div(X1, X0))</t>
+  </si>
+  <si>
+    <t>div(mul(X1, X1), div(X0, 0.575))</t>
+  </si>
+  <si>
+    <t>Ea = 0.575*Ebind^2/Ec</t>
+  </si>
+  <si>
+    <t>div(mul(X1, X1), div(X0, 0.565))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ea = 0.565*Ebind^2/Ec </t>
+  </si>
+  <si>
+    <t>mul(X1, div(X1, div(X0, 0.570)))</t>
+  </si>
+  <si>
+    <t>Ea = 0.570*Ebind^2/Ec</t>
+  </si>
+  <si>
+    <t>Ea = Ebind^2/Ec - Ebind^1.5/Ec</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -92,15 +100,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -108,12 +122,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,137 +424,182 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A3" sqref="A3:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1"/>
+    <col min="6" max="6" width="46.28515625" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.24562609444241901</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.29247017528039898</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.92535315589959199</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.97026915309521899</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.20536378156219101</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.281865435645832</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.94012573581764602</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.97450749804470804</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.24216363207226699</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.281280969855909</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.92749789192948695</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.970269153095218</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.239229456859686</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.274294423665006</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.92793582340777603</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.97026915309521899</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>0.241830740515589</v>
-      </c>
-      <c r="C4">
-        <v>0.280368850599724</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>0.22762521830361801</v>
-      </c>
-      <c r="C5">
-        <v>0.27178776427967599</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>0.23733546653780099</v>
-      </c>
-      <c r="C6">
-        <v>0.271092913298069</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>0.23627770515531701</v>
-      </c>
-      <c r="C7">
-        <v>0.26976939166883401</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>0.242494982354273</v>
-      </c>
-      <c r="C8">
-        <v>0.28221832474858699</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="B8" s="2">
+        <v>0.24063047558300699</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.277330878192594</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.927884601973892</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.97026915309521899</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="G8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update graphs for manuscript
</commit_message>
<xml_diff>
--- a/gp/Ea_gp_models.xlsx
+++ b/gp/Ea_gp_models.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D25218E-29ED-9E46-8B8B-555BA81EB1BB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="645" yWindow="2715" windowWidth="23730" windowHeight="11385"/>
+    <workbookView xWindow="11040" yWindow="3180" windowWidth="23740" windowHeight="11380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">Model </t>
   </si>
@@ -45,9 +46,6 @@
     <t>MAE (eV)</t>
   </si>
   <si>
-    <t>RMSE (eV)</t>
-  </si>
-  <si>
     <t>r2</t>
   </si>
   <si>
@@ -82,12 +80,30 @@
   </si>
   <si>
     <t>Ea = Ebind^2/Ec - Ebind^1.5/Ec</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>Testing RMSE (eV)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -100,8 +116,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -148,10 +165,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -433,24 +456,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="46.28515625" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="6" max="6" width="46.33203125" customWidth="1"/>
+    <col min="7" max="7" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -458,7 +481,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -466,7 +489,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,13 +497,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>1</v>
@@ -490,9 +513,9 @@
       </c>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>1</v>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="B4" s="2">
         <v>0.24562609444241901</v>
@@ -507,16 +530,16 @@
         <v>0.97026915309521899</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>2</v>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B5" s="2">
         <v>0.20536378156219101</v>
@@ -531,16 +554,16 @@
         <v>0.97450749804470804</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>3</v>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B6" s="2">
         <v>0.24216363207226699</v>
@@ -555,16 +578,16 @@
         <v>0.970269153095218</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>4</v>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B7" s="2">
         <v>0.239229456859686</v>
@@ -579,34 +602,34 @@
         <v>0.97026915309521899</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>5</v>
-      </c>
-      <c r="B8" s="3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="5">
         <v>0.24063047558300699</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="5">
         <v>0.277330878192594</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="5">
         <v>0.927884601973892</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="5">
         <v>0.97026915309521899</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>18</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="H8" s="1"/>
     </row>

</xml_diff>